<commit_message>
analysis of identity criteria for topgraphic objects
Signed-off-by: Pawel Garbacz <pawel.garbacz@makolab.com>
</commit_message>
<xml_diff>
--- a/kryteria_tożsamości_dla_obiektów_topgraficznych.xlsx
+++ b/kryteria_tożsamości_dla_obiektów_topgraficznych.xlsx
@@ -8,21 +8,36 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\ihpan\urbanonto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D8713C7-C6A3-4E41-9336-3B27FB068FC1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CD45B06-E4A9-41E0-8357-CAD05584E8D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="17640" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="typy" sheetId="1" r:id="rId1"/>
     <sheet name="referencje" sheetId="2" r:id="rId2"/>
     <sheet name="manifestacje" sheetId="3" r:id="rId3"/>
+    <sheet name="szpital_bozego_ciala" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">szpital_bozego_ciala!$A$1:$L$20</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="253">
   <si>
     <t>label</t>
   </si>
@@ -694,6 +709,93 @@
   </si>
   <si>
     <t>NZOZ Limfa</t>
+  </si>
+  <si>
+    <t>czas_od</t>
+  </si>
+  <si>
+    <t>czas_do</t>
+  </si>
+  <si>
+    <t>Szpital Bożego Ciała</t>
+  </si>
+  <si>
+    <t>Kaplica Bożego Ciała</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>kaplica</t>
+  </si>
+  <si>
+    <t>kościół</t>
+  </si>
+  <si>
+    <t>typ_nazwa</t>
+  </si>
+  <si>
+    <t>typ_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kaplica Trójcy Świętej </t>
+  </si>
+  <si>
+    <t>jest_częścią_obiekt_id</t>
+  </si>
+  <si>
+    <t>jest_częścią_obiekt_nazwa</t>
+  </si>
+  <si>
+    <t>Trzecia Brama Świdnicka</t>
+  </si>
+  <si>
+    <t>Komandoria</t>
+  </si>
+  <si>
+    <t>Kompleks Klasztorny Bożego Ciała</t>
+  </si>
+  <si>
+    <t>Kościół Bożego Ciała</t>
+  </si>
+  <si>
+    <t>pochodzi_od_obiektu_id</t>
+  </si>
+  <si>
+    <t>pochodzi_od_obiektu_nazwa</t>
+  </si>
+  <si>
+    <t>Szpital Trójcy Świętej</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kościół Trójcy Świętej </t>
+  </si>
+  <si>
+    <t>[null]</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>ABD</t>
+  </si>
+  <si>
+    <t>ABCD</t>
+  </si>
+  <si>
+    <t>ABCDEF</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>G</t>
   </si>
 </sst>
 </file>
@@ -701,7 +803,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -753,12 +855,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -1074,1089 +1180,1723 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E206"/>
+  <dimension ref="A1:F208"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <pane ySplit="1" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B209" sqref="B209"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="43.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="43.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>99</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>211</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>168</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>211</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>70</v>
+      </c>
+      <c r="B71" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>71</v>
+      </c>
+      <c r="B72" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>72</v>
+      </c>
+      <c r="B73" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>73</v>
+      </c>
+      <c r="B74" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>74</v>
+      </c>
+      <c r="B75" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>75</v>
+      </c>
+      <c r="B76" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>76</v>
+      </c>
+      <c r="B77" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>77</v>
+      </c>
+      <c r="B78" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>78</v>
+      </c>
+      <c r="B79" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>79</v>
+      </c>
+      <c r="B80" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>80</v>
+      </c>
+      <c r="B81" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>81</v>
+      </c>
+      <c r="B82" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>82</v>
+      </c>
+      <c r="B83" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>83</v>
+      </c>
+      <c r="B84" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>84</v>
+      </c>
+      <c r="B85" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>85</v>
+      </c>
+      <c r="B86" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>86</v>
+      </c>
+      <c r="B87" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>87</v>
+      </c>
+      <c r="B88" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>88</v>
+      </c>
+      <c r="B89" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>89</v>
+      </c>
+      <c r="B90" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>90</v>
+      </c>
+      <c r="B91" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>91</v>
+      </c>
+      <c r="B92" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>92</v>
+      </c>
+      <c r="B93" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>93</v>
+      </c>
+      <c r="B94" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>94</v>
+      </c>
+      <c r="B95" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>95</v>
+      </c>
+      <c r="B96" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>96</v>
+      </c>
+      <c r="B97" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>97</v>
+      </c>
+      <c r="B98" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>98</v>
+      </c>
+      <c r="B99" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>99</v>
+      </c>
+      <c r="B100" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>100</v>
+      </c>
+      <c r="B101" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>101</v>
+      </c>
+      <c r="B102" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>102</v>
+      </c>
+      <c r="B103" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>103</v>
+      </c>
+      <c r="B104" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>104</v>
+      </c>
+      <c r="B105" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>105</v>
+      </c>
+      <c r="B106" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>106</v>
+      </c>
+      <c r="B107" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>107</v>
+      </c>
+      <c r="B108" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>108</v>
+      </c>
+      <c r="B109" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>109</v>
+      </c>
+      <c r="B110" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>110</v>
+      </c>
+      <c r="B111" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>111</v>
+      </c>
+      <c r="B112" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>112</v>
+      </c>
+      <c r="B113" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>113</v>
+      </c>
+      <c r="B114" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>114</v>
+      </c>
+      <c r="B115" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>115</v>
+      </c>
+      <c r="B116" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>116</v>
+      </c>
+      <c r="B117" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>117</v>
+      </c>
+      <c r="B118" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>118</v>
+      </c>
+      <c r="B119" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>119</v>
+      </c>
+      <c r="B120" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>120</v>
+      </c>
+      <c r="B121" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>121</v>
+      </c>
+      <c r="B122" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>122</v>
+      </c>
+      <c r="B123" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>123</v>
+      </c>
+      <c r="B124" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>124</v>
+      </c>
+      <c r="B125" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>125</v>
+      </c>
+      <c r="B126" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>126</v>
+      </c>
+      <c r="B127" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>127</v>
+      </c>
+      <c r="B128" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>128</v>
+      </c>
+      <c r="B129" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>129</v>
+      </c>
+      <c r="B130" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>130</v>
+      </c>
+      <c r="B131" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>131</v>
+      </c>
+      <c r="B132" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>132</v>
+      </c>
+      <c r="B133" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>133</v>
+      </c>
+      <c r="B134" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>134</v>
+      </c>
+      <c r="B135" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <v>135</v>
+      </c>
+      <c r="B136" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>136</v>
+      </c>
+      <c r="B137" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>137</v>
+      </c>
+      <c r="B138" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>138</v>
+      </c>
+      <c r="B139" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <v>139</v>
+      </c>
+      <c r="B140" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>140</v>
+      </c>
+      <c r="B141" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <v>141</v>
+      </c>
+      <c r="B142" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <v>142</v>
+      </c>
+      <c r="B143" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A144" t="s">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144">
+        <v>143</v>
+      </c>
+      <c r="B144" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <v>144</v>
+      </c>
+      <c r="B145" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A146" t="s">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146">
+        <v>145</v>
+      </c>
+      <c r="B146" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A147" t="s">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A147">
+        <v>146</v>
+      </c>
+      <c r="B147" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A148" t="s">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A148">
+        <v>147</v>
+      </c>
+      <c r="B148" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A149" t="s">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A149">
+        <v>148</v>
+      </c>
+      <c r="B149" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A150" t="s">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A150">
+        <v>149</v>
+      </c>
+      <c r="B150" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A151" t="s">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A151">
+        <v>150</v>
+      </c>
+      <c r="B151" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A152" t="s">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A152">
+        <v>151</v>
+      </c>
+      <c r="B152" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A153" t="s">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A153">
+        <v>152</v>
+      </c>
+      <c r="B153" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A154" t="s">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A154">
+        <v>153</v>
+      </c>
+      <c r="B154" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A155" t="s">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A155">
+        <v>154</v>
+      </c>
+      <c r="B155" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A156" t="s">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A156">
+        <v>155</v>
+      </c>
+      <c r="B156" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A157" t="s">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A157">
+        <v>156</v>
+      </c>
+      <c r="B157" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A158" t="s">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A158">
+        <v>157</v>
+      </c>
+      <c r="B158" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A159" t="s">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A159">
+        <v>158</v>
+      </c>
+      <c r="B159" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A160" t="s">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A160">
+        <v>159</v>
+      </c>
+      <c r="B160" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A161" t="s">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A161">
+        <v>160</v>
+      </c>
+      <c r="B161" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A162" t="s">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A162">
+        <v>161</v>
+      </c>
+      <c r="B162" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A163" t="s">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A163">
+        <v>162</v>
+      </c>
+      <c r="B163" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A164" t="s">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A164">
+        <v>163</v>
+      </c>
+      <c r="B164" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A165" t="s">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A165">
+        <v>164</v>
+      </c>
+      <c r="B165" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A166" t="s">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A166">
+        <v>165</v>
+      </c>
+      <c r="B166" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A167" t="s">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A167">
+        <v>166</v>
+      </c>
+      <c r="B167" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A168" t="s">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A168">
+        <v>167</v>
+      </c>
+      <c r="B168" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A169" t="s">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A169">
+        <v>168</v>
+      </c>
+      <c r="B169" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A170" t="s">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A170">
+        <v>169</v>
+      </c>
+      <c r="B170" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A171" t="s">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A171">
+        <v>170</v>
+      </c>
+      <c r="B171" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A172" t="s">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A172">
+        <v>171</v>
+      </c>
+      <c r="B172" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A173" t="s">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A173">
+        <v>172</v>
+      </c>
+      <c r="B173" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A174" t="s">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A174">
+        <v>173</v>
+      </c>
+      <c r="B174" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A175" t="s">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A175">
+        <v>174</v>
+      </c>
+      <c r="B175" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A176" t="s">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A176">
+        <v>175</v>
+      </c>
+      <c r="B176" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A177" t="s">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A177">
+        <v>176</v>
+      </c>
+      <c r="B177" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A178" t="s">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A178">
+        <v>177</v>
+      </c>
+      <c r="B178" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A179" t="s">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A179">
+        <v>178</v>
+      </c>
+      <c r="B179" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A180" t="s">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A180">
+        <v>179</v>
+      </c>
+      <c r="B180" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A181" t="s">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A181">
+        <v>180</v>
+      </c>
+      <c r="B181" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A182" t="s">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A182">
+        <v>181</v>
+      </c>
+      <c r="B182" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A183" t="s">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A183">
+        <v>182</v>
+      </c>
+      <c r="B183" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A184" t="s">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A184">
+        <v>183</v>
+      </c>
+      <c r="B184" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A185" t="s">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A185">
+        <v>184</v>
+      </c>
+      <c r="B185" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A186" t="s">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A186">
+        <v>185</v>
+      </c>
+      <c r="B186" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A187" t="s">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A187">
+        <v>186</v>
+      </c>
+      <c r="B187" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A188" t="s">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A188">
+        <v>187</v>
+      </c>
+      <c r="B188" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A189" t="s">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A189">
+        <v>188</v>
+      </c>
+      <c r="B189" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A190" t="s">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A190">
+        <v>189</v>
+      </c>
+      <c r="B190" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A191" t="s">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A191">
+        <v>190</v>
+      </c>
+      <c r="B191" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A192" t="s">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A192">
+        <v>191</v>
+      </c>
+      <c r="B192" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A193" t="s">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A193">
+        <v>192</v>
+      </c>
+      <c r="B193" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A194" t="s">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A194">
+        <v>193</v>
+      </c>
+      <c r="B194" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A195" t="s">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A195">
+        <v>194</v>
+      </c>
+      <c r="B195" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A196" t="s">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A196">
+        <v>195</v>
+      </c>
+      <c r="B196" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A197" t="s">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A197">
+        <v>196</v>
+      </c>
+      <c r="B197" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A198" t="s">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A198">
+        <v>197</v>
+      </c>
+      <c r="B198" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A199" t="s">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A199">
+        <v>198</v>
+      </c>
+      <c r="B199" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A200" t="s">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A200">
+        <v>199</v>
+      </c>
+      <c r="B200" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A201" t="s">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A201">
+        <v>200</v>
+      </c>
+      <c r="B201" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A202" t="s">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A202">
+        <v>201</v>
+      </c>
+      <c r="B202" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A203" t="s">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A203">
+        <v>202</v>
+      </c>
+      <c r="B203" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A204" t="s">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A204">
+        <v>203</v>
+      </c>
+      <c r="B204" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A205" t="s">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A205">
+        <v>204</v>
+      </c>
+      <c r="B205" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A206" t="s">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A206">
+        <v>205</v>
+      </c>
+      <c r="B206" t="s">
         <v>115</v>
       </c>
     </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A207">
+        <v>206</v>
+      </c>
+      <c r="B207" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A208">
+        <v>207</v>
+      </c>
+      <c r="B208" t="s">
+        <v>230</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A206">
-    <sortCondition ref="A2:A206"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:B206">
+    <sortCondition ref="B2:B206"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A3DD3AA4-3D61-4750-9A8B-348708767AD2}">
           <x14:formula1>
             <xm:f>referencje!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:E206</xm:sqref>
+          <xm:sqref>C2:F206</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2196,7 +2936,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B61B91CF-E87E-4C17-9A4B-A6CCF6B63099}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
@@ -2484,4 +3224,790 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B79EF5B2-5AA4-49FA-A93F-79119EBA02A0}">
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:L20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.85546875" customWidth="1"/>
+    <col min="12" max="12" width="27.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="7">
+        <v>1317</v>
+      </c>
+      <c r="D2" s="6">
+        <v>1337</v>
+      </c>
+      <c r="E2" t="s">
+        <v>226</v>
+      </c>
+      <c r="F2">
+        <v>174</v>
+      </c>
+      <c r="G2" t="str">
+        <f>VLOOKUP(F2,typy!A:B,2,FALSE)</f>
+        <v>szpital przednowoczesny</v>
+      </c>
+      <c r="H2" t="s">
+        <v>248</v>
+      </c>
+      <c r="J2" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(I2,B:E,4,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="L2" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(K2,B:E,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" s="7">
+        <v>1317</v>
+      </c>
+      <c r="D3" s="6">
+        <v>1354</v>
+      </c>
+      <c r="E3" t="s">
+        <v>227</v>
+      </c>
+      <c r="F3">
+        <v>206</v>
+      </c>
+      <c r="G3" t="str">
+        <f>VLOOKUP(F3,typy!A:B,2,FALSE)</f>
+        <v>kaplica</v>
+      </c>
+      <c r="H3" t="s">
+        <v>245</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(I3,B:E,4,FALSE),"")</f>
+        <v>Szpital Bożego Ciała</v>
+      </c>
+      <c r="L3" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(K3,B:E,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" s="6">
+        <v>1337</v>
+      </c>
+      <c r="D4" s="6">
+        <v>1826</v>
+      </c>
+      <c r="E4" t="s">
+        <v>238</v>
+      </c>
+      <c r="F4">
+        <v>202</v>
+      </c>
+      <c r="G4" t="str">
+        <f>VLOOKUP(F4,typy!A:B,2,FALSE)</f>
+        <v>zespół sakralny lub klasztorny</v>
+      </c>
+      <c r="H4" t="s">
+        <v>249</v>
+      </c>
+      <c r="J4" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(I4,B:E,4,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="L4" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(K4,B:E,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" s="6">
+        <v>1337</v>
+      </c>
+      <c r="D5" s="6">
+        <v>1450</v>
+      </c>
+      <c r="E5" t="s">
+        <v>237</v>
+      </c>
+      <c r="F5">
+        <v>81</v>
+      </c>
+      <c r="G5" t="str">
+        <f>VLOOKUP(F5,typy!A:B,2,FALSE)</f>
+        <v>klasztor</v>
+      </c>
+      <c r="H5" t="s">
+        <v>246</v>
+      </c>
+      <c r="I5">
+        <v>3</v>
+      </c>
+      <c r="J5" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(I5,B:E,4,FALSE),"")</f>
+        <v>Kompleks Klasztorny Bożego Ciała</v>
+      </c>
+      <c r="L5" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(K5,B:E,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" s="6">
+        <v>1337</v>
+      </c>
+      <c r="D6" s="6">
+        <v>1354</v>
+      </c>
+      <c r="E6" t="s">
+        <v>226</v>
+      </c>
+      <c r="F6">
+        <v>174</v>
+      </c>
+      <c r="G6" t="str">
+        <f>VLOOKUP(F6,typy!A:B,2,FALSE)</f>
+        <v>szpital przednowoczesny</v>
+      </c>
+      <c r="H6" t="s">
+        <v>248</v>
+      </c>
+      <c r="I6">
+        <v>3</v>
+      </c>
+      <c r="J6" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(I6,B:E,4,FALSE),"")</f>
+        <v>Kompleks Klasztorny Bożego Ciała</v>
+      </c>
+      <c r="L6" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(K6,B:E,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7" s="6">
+        <v>1354</v>
+      </c>
+      <c r="D7" s="6">
+        <v>1450</v>
+      </c>
+      <c r="E7" t="s">
+        <v>239</v>
+      </c>
+      <c r="F7">
+        <v>207</v>
+      </c>
+      <c r="G7" t="str">
+        <f>VLOOKUP(F7,typy!A:B,2,FALSE)</f>
+        <v>kościół</v>
+      </c>
+      <c r="H7" t="s">
+        <v>245</v>
+      </c>
+      <c r="J7" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(I7,B:E,4,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="K7">
+        <v>2</v>
+      </c>
+      <c r="L7" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(K7,B:E,4,FALSE),"")</f>
+        <v>Kaplica Bożego Ciała</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" s="6">
+        <v>1354</v>
+      </c>
+      <c r="D8" s="6">
+        <v>1466</v>
+      </c>
+      <c r="E8" t="s">
+        <v>226</v>
+      </c>
+      <c r="F8">
+        <v>174</v>
+      </c>
+      <c r="G8" t="str">
+        <f>VLOOKUP(F8,typy!A:B,2,FALSE)</f>
+        <v>szpital przednowoczesny</v>
+      </c>
+      <c r="H8" t="s">
+        <v>248</v>
+      </c>
+      <c r="J8" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(I8,B:E,4,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="L8" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(K8,B:E,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>6</v>
+      </c>
+      <c r="C9" s="6">
+        <v>1366</v>
+      </c>
+      <c r="D9" s="6">
+        <v>1466</v>
+      </c>
+      <c r="E9" t="s">
+        <v>233</v>
+      </c>
+      <c r="F9">
+        <v>206</v>
+      </c>
+      <c r="G9" t="str">
+        <f>VLOOKUP(F9,typy!A:B,2,FALSE)</f>
+        <v>kaplica</v>
+      </c>
+      <c r="H9" t="s">
+        <v>247</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(I9,B:E,4,FALSE),"")</f>
+        <v>Szpital Bożego Ciała</v>
+      </c>
+      <c r="L9" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(K9,B:E,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>7</v>
+      </c>
+      <c r="C10" s="6">
+        <v>1450</v>
+      </c>
+      <c r="D10" s="6">
+        <v>2020</v>
+      </c>
+      <c r="E10" t="s">
+        <v>236</v>
+      </c>
+      <c r="F10">
+        <v>17</v>
+      </c>
+      <c r="G10" t="str">
+        <f>VLOOKUP(F10,typy!A:B,2,FALSE)</f>
+        <v>brama miejska</v>
+      </c>
+      <c r="H10" t="s">
+        <v>250</v>
+      </c>
+      <c r="J10" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(I10,B:E,4,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="L10" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(K10,B:E,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="C11" s="6">
+        <v>1450</v>
+      </c>
+      <c r="D11" s="6">
+        <v>1826</v>
+      </c>
+      <c r="E11" t="s">
+        <v>237</v>
+      </c>
+      <c r="F11">
+        <v>81</v>
+      </c>
+      <c r="G11" t="str">
+        <f>VLOOKUP(F11,typy!A:B,2,FALSE)</f>
+        <v>klasztor</v>
+      </c>
+      <c r="H11" t="s">
+        <v>246</v>
+      </c>
+      <c r="I11">
+        <v>7</v>
+      </c>
+      <c r="J11" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(I11,B:E,4,FALSE),"")</f>
+        <v>Trzecia Brama Świdnicka</v>
+      </c>
+      <c r="L11" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(K11,B:E,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>5</v>
+      </c>
+      <c r="C12" s="6">
+        <v>1450</v>
+      </c>
+      <c r="D12" s="6">
+        <v>1758</v>
+      </c>
+      <c r="E12" t="s">
+        <v>239</v>
+      </c>
+      <c r="F12">
+        <v>207</v>
+      </c>
+      <c r="G12" t="str">
+        <f>VLOOKUP(F12,typy!A:B,2,FALSE)</f>
+        <v>kościół</v>
+      </c>
+      <c r="H12" t="s">
+        <v>245</v>
+      </c>
+      <c r="I12">
+        <v>7</v>
+      </c>
+      <c r="J12" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(I12,B:E,4,FALSE),"")</f>
+        <v>Trzecia Brama Świdnicka</v>
+      </c>
+      <c r="L12" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(K12,B:E,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>6</v>
+      </c>
+      <c r="C13" s="6">
+        <v>1466</v>
+      </c>
+      <c r="D13" s="6">
+        <v>1867</v>
+      </c>
+      <c r="E13" t="s">
+        <v>233</v>
+      </c>
+      <c r="F13">
+        <v>76</v>
+      </c>
+      <c r="G13" t="str">
+        <f>VLOOKUP(F13,typy!A:B,2,FALSE)</f>
+        <v>kaplica wolnostojąca</v>
+      </c>
+      <c r="H13" t="s">
+        <v>247</v>
+      </c>
+      <c r="J13" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(I13,B:E,4,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="L13" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(K13,B:E,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" s="6">
+        <v>1466</v>
+      </c>
+      <c r="D14" s="6">
+        <v>1867</v>
+      </c>
+      <c r="E14" t="s">
+        <v>242</v>
+      </c>
+      <c r="F14">
+        <v>174</v>
+      </c>
+      <c r="G14" t="str">
+        <f>VLOOKUP(F14,typy!A:B,2,FALSE)</f>
+        <v>szpital przednowoczesny</v>
+      </c>
+      <c r="H14" t="s">
+        <v>248</v>
+      </c>
+      <c r="J14" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(I14,B:E,4,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="L14" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(K14,B:E,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>15</v>
+      </c>
+      <c r="B15">
+        <v>8</v>
+      </c>
+      <c r="C15" s="6">
+        <v>1758</v>
+      </c>
+      <c r="D15" s="6">
+        <v>1813</v>
+      </c>
+      <c r="E15" t="s">
+        <v>244</v>
+      </c>
+      <c r="F15">
+        <v>89</v>
+      </c>
+      <c r="G15" t="str">
+        <f>VLOOKUP(F15,typy!A:B,2,FALSE)</f>
+        <v>magazyn</v>
+      </c>
+      <c r="H15" t="s">
+        <v>245</v>
+      </c>
+      <c r="J15" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(I15,B:E,4,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="K15">
+        <v>5</v>
+      </c>
+      <c r="L15" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(K15,B:E,4,FALSE),"")</f>
+        <v>Kościół Bożego Ciała</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>16</v>
+      </c>
+      <c r="B16">
+        <v>9</v>
+      </c>
+      <c r="C16" s="6">
+        <v>1813</v>
+      </c>
+      <c r="D16" s="6">
+        <v>1945</v>
+      </c>
+      <c r="E16" t="s">
+        <v>239</v>
+      </c>
+      <c r="F16">
+        <v>173</v>
+      </c>
+      <c r="G16" t="str">
+        <f>VLOOKUP(F16,typy!A:B,2,FALSE)</f>
+        <v>szpital</v>
+      </c>
+      <c r="H16" t="s">
+        <v>245</v>
+      </c>
+      <c r="J16" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(I16,B:E,4,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="K16">
+        <v>8</v>
+      </c>
+      <c r="L16" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(K16,B:E,4,FALSE),"")</f>
+        <v>[null]</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>17</v>
+      </c>
+      <c r="B17">
+        <v>10</v>
+      </c>
+      <c r="C17" s="6">
+        <v>1867</v>
+      </c>
+      <c r="D17" s="6">
+        <v>1945</v>
+      </c>
+      <c r="E17" t="s">
+        <v>242</v>
+      </c>
+      <c r="F17">
+        <v>173</v>
+      </c>
+      <c r="G17" t="str">
+        <f>VLOOKUP(F17,typy!A:B,2,FALSE)</f>
+        <v>szpital</v>
+      </c>
+      <c r="H17" t="s">
+        <v>251</v>
+      </c>
+      <c r="J17" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(I17,B:E,4,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="L17" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(K17,B:E,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>18</v>
+      </c>
+      <c r="B18">
+        <v>11</v>
+      </c>
+      <c r="C18" s="6">
+        <v>1867</v>
+      </c>
+      <c r="D18" s="6">
+        <v>1945</v>
+      </c>
+      <c r="E18" t="s">
+        <v>243</v>
+      </c>
+      <c r="F18">
+        <v>207</v>
+      </c>
+      <c r="G18" t="str">
+        <f>VLOOKUP(F18,typy!A:B,2,FALSE)</f>
+        <v>kościół</v>
+      </c>
+      <c r="H18" t="s">
+        <v>252</v>
+      </c>
+      <c r="J18" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(I18,B:E,4,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="L18" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(K18,B:E,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>19</v>
+      </c>
+      <c r="B19">
+        <v>12</v>
+      </c>
+      <c r="C19" s="6">
+        <v>1945</v>
+      </c>
+      <c r="D19" s="6">
+        <v>1956</v>
+      </c>
+      <c r="E19" t="s">
+        <v>239</v>
+      </c>
+      <c r="F19">
+        <v>145</v>
+      </c>
+      <c r="G19" t="str">
+        <f>VLOOKUP(F19,typy!A:B,2,FALSE)</f>
+        <v>ruina zabytkowa</v>
+      </c>
+      <c r="H19" t="s">
+        <v>245</v>
+      </c>
+      <c r="J19" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(I19,B:E,4,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="K19">
+        <v>9</v>
+      </c>
+      <c r="L19" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(K19,B:E,4,FALSE),"")</f>
+        <v>Kościół Bożego Ciała</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>20</v>
+      </c>
+      <c r="B20">
+        <v>13</v>
+      </c>
+      <c r="C20" s="6">
+        <v>1956</v>
+      </c>
+      <c r="D20" s="6">
+        <v>2020</v>
+      </c>
+      <c r="E20" t="s">
+        <v>239</v>
+      </c>
+      <c r="F20">
+        <v>207</v>
+      </c>
+      <c r="G20" t="str">
+        <f>VLOOKUP(F20,typy!A:B,2,FALSE)</f>
+        <v>kościół</v>
+      </c>
+      <c r="H20" t="s">
+        <v>245</v>
+      </c>
+      <c r="J20" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(I20,B:E,4,FALSE),"")</f>
+        <v/>
+      </c>
+      <c r="K20">
+        <v>12</v>
+      </c>
+      <c r="L20" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(K20,B:E,4,FALSE),"")</f>
+        <v>Kościół Bożego Ciała</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:L20" xr:uid="{007D034A-544A-4E1F-95BF-2B8F82E1EB42}">
+    <filterColumn colId="7">
+      <filters>
+        <filter val="B"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D18CA4F6-82FD-4806-9DD0-2FEF82F31352}">
+          <x14:formula1>
+            <xm:f>typy!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>F2:F1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>